<commit_message>
changed .related into extension
</commit_message>
<xml_diff>
--- a/Mappings/OutcomeOfCare - STU3.xlsx
+++ b/Mappings/OutcomeOfCare - STU3.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="525" windowWidth="20775" windowHeight="9405" activeTab="3"/>
+    <workbookView xWindow="270" yWindow="525" windowWidth="20775" windowHeight="9405" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Information Model" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Research" sheetId="6" r:id="rId4"/>
     <sheet name="Data" sheetId="4" r:id="rId5"/>
     <sheet name="Terms of Use" sheetId="5" r:id="rId6"/>
   </sheets>
@@ -348,9 +348,6 @@
     <t>.valueString</t>
   </si>
   <si>
-    <t>.related.target where target profile is http://nictiz.nl/fhir/StructureDefinition/zib-NursingIntervention</t>
-  </si>
-  <si>
     <t>.measurementValue, extension where valueReference target profile is http://nictiz.nl/fhir/StructureDefinition/zib-GeneralMeasurement</t>
   </si>
   <si>
@@ -412,6 +409,9 @@
   </si>
   <si>
     <t>outcome of (-nursing intervention, -care)</t>
+  </si>
+  <si>
+    <t>.nursingIntervention, extension where target profile is http://nictiz.nl/fhir/StructureDefinition/zib-NursingIntervention</t>
   </si>
 </sst>
 </file>
@@ -585,9 +585,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -600,6 +597,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9382,10 +9382,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
@@ -9599,8 +9599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9611,127 +9611,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="A2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="A3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
-        <v>120</v>
+      <c r="A4" s="16" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="20" t="s">
-        <v>119</v>
+      <c r="A5" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="20" t="s">
-        <v>119</v>
+      <c r="A6" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="20" t="s">
-        <v>119</v>
+      <c r="A7" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="20" t="s">
-        <v>119</v>
+      <c r="A8" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="19" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="17" t="s">
-        <v>125</v>
+      <c r="A9" s="16" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="20" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>127</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17" t="s">
-        <v>127</v>
+      <c r="A12" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -13777,8 +13777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -13791,7 +13791,7 @@
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="18" width="30" style="17" customWidth="1"/>
+    <col min="16" max="18" width="30" style="16" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13828,13 +13828,13 @@
       <c r="O2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="R2" s="17" t="s">
         <v>106</v>
       </c>
       <c r="S2" s="1" t="s">
@@ -13866,11 +13866,11 @@
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
       <c r="S3" s="4"/>
     </row>
     <row r="4" spans="2:19" ht="63.75">
@@ -13904,13 +13904,13 @@
         <v>80</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16" t="s">
-        <v>112</v>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="63.75">
@@ -13942,13 +13942,13 @@
       <c r="O5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="P5" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
+      <c r="P5" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
       <c r="S5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:19" ht="51">
@@ -13980,13 +13980,13 @@
       <c r="O6" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="51">
@@ -14018,11 +14018,11 @@
       <c r="O7" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P7" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
+      <c r="P7" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
       <c r="S7" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated mappings in OutcomeOfCare
</commit_message>
<xml_diff>
--- a/Mappings/OutcomeOfCare - STU3.xlsx
+++ b/Mappings/OutcomeOfCare - STU3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nictiz-stu3-zib2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E3AB9D-E85A-476F-ADAE-98F22A10D63E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="525" windowWidth="20775" windowHeight="9405" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="525" windowWidth="20775" windowHeight="9405" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="135">
   <si>
     <t>Subject</t>
   </si>
@@ -354,12 +353,6 @@
     <t>.valueString</t>
   </si>
   <si>
-    <t>.measurementValue, extension where valueReference target profile is http://nictiz.nl/fhir/StructureDefinition/zib-GeneralMeasurement</t>
-  </si>
-  <si>
-    <t>.healthCondition, extension where valueReference target profile is http://nictiz.nl/fhir/StructureDefinition/zib-FunctionOrMentalStatus</t>
-  </si>
-  <si>
     <t>Checkbox searched for existing profiles / implementation on:</t>
   </si>
   <si>
@@ -414,19 +407,34 @@
     <t>outcome of (-nursing intervention, -care)</t>
   </si>
   <si>
-    <t>.nursingIntervention, extension where target profile is http://nictiz.nl/fhir/StructureDefinition/zib-NursingIntervention</t>
-  </si>
-  <si>
     <t>In Goal resource: "Goals are often evaluated using Observations."</t>
   </si>
   <si>
     <t>Only one of these three options must be present</t>
   </si>
+  <si>
+    <t>Observation (HCIM: FunctionalOrMentalStatus)</t>
+  </si>
+  <si>
+    <t>Observation (HCIM: GeneralMeasurement)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation.extension.partOf  </t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Mock element from R4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -489,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -549,11 +557,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -607,6 +626,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -13828,23 +13850,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -13880,23 +13885,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -14072,7 +14060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14181,7 +14169,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -14192,7 +14180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14399,7 +14387,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14418,7 +14406,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14434,19 +14422,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>115</v>
       </c>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
@@ -14455,14 +14443,14 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E2" s="16"/>
       <c r="G2" s="18"/>
@@ -14474,7 +14462,7 @@
       <c r="A3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E3" s="16"/>
       <c r="G3" s="18"/>
@@ -14484,79 +14472,79 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -18600,11 +18588,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18616,10 +18604,10 @@
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="75" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="30" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
     <col min="16" max="16" width="30" style="16" customWidth="1"/>
-    <col min="17" max="17" width="21.140625" style="16" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" style="16" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" style="16" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" style="16" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18735,13 +18723,15 @@
       <c r="P4" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="Q4" s="15"/>
+      <c r="Q4" s="15" t="s">
+        <v>132</v>
+      </c>
       <c r="R4" s="15"/>
       <c r="S4" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>81</v>
@@ -18771,15 +18761,17 @@
         <v>86</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
-      <c r="Q5" s="15"/>
+      <c r="Q5" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="R5" s="15"/>
       <c r="S5" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="6" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>87</v>
@@ -18809,15 +18801,17 @@
         <v>91</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
-      <c r="Q6" s="15"/>
+      <c r="Q6" s="15" t="s">
+        <v>133</v>
+      </c>
       <c r="R6" s="15"/>
       <c r="S6" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:19" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>92</v>
@@ -18847,17 +18841,21 @@
         <v>97</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="2"/>
+      <c r="Q7" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="S7" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O5" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="O6" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="O7" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="O5" r:id="rId1"/>
+    <hyperlink ref="O6" r:id="rId2"/>
+    <hyperlink ref="O7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -18867,7 +18865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
updated OutcomeOfCare: instead of Observation, derived profile on TextResult. Added reference to Nursingintervention.
</commit_message>
<xml_diff>
--- a/Mappings/OutcomeOfCare - STU3.xlsx
+++ b/Mappings/OutcomeOfCare - STU3.xlsx
@@ -413,38 +413,30 @@
     <t>Observation (HCIM: GeneralMeasurement)</t>
   </si>
   <si>
-    <t>equal</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Procedure / Careplan.activity</t>
+    <t>CarePlan.activity:nursingIntervention.outcomeCodeableConcept Or derived profile on zib-TextResult.</t>
   </si>
   <si>
     <t xml:space="preserve">** OutcomeOfCare
-Maps to CarePlan / or Procedure and referenced resources
-Add mappings to 
-* CarePlan
-* NursingIntervention
-* Procedure
-* TextResult
-* GeneralMeasurement
-* FunctionalOrMentalStatus
 </t>
   </si>
   <si>
-    <t>DiagnosticReport.conclusion (HCIM Textresult)</t>
+    <t>CarePlan  / DiagnosticResult</t>
   </si>
   <si>
-    <t>CarePlan  / Procedure</t>
+    <t>Careplan.activity / DiagnosticReport.extention.partOf</t>
+  </si>
+  <si>
+    <t>Maybe not the most suitable extension.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -634,10 +626,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -14074,13 +14066,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -14088,7 +14080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -14096,7 +14088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -14104,7 +14096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -14112,7 +14104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -14120,7 +14112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -14128,7 +14120,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -14136,7 +14128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -14144,7 +14136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -14152,7 +14144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -14160,7 +14152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="51">
+    <row r="12" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
@@ -14168,7 +14160,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25.5">
+    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>57</v>
       </c>
@@ -14194,19 +14186,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="21"/>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -14214,7 +14206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -14222,7 +14214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -14230,7 +14222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -14238,7 +14230,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -14246,7 +14238,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -14254,13 +14246,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -14268,13 +14260,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -14282,13 +14274,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -14296,7 +14288,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -14304,7 +14296,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
@@ -14312,7 +14304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -14320,7 +14312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
@@ -14328,7 +14320,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -14336,7 +14328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -14344,7 +14336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -14352,7 +14344,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
@@ -14360,7 +14352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
@@ -14368,7 +14360,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
@@ -14376,7 +14368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
@@ -14403,9 +14395,9 @@
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -14422,14 +14414,14 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.28515625" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
     <col min="4" max="4" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>107</v>
       </c>
@@ -14450,7 +14442,7 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>112</v>
       </c>
@@ -14467,7 +14459,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="19" t="s">
@@ -14479,7 +14471,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>114</v>
       </c>
@@ -14487,7 +14479,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>115</v>
       </c>
@@ -14496,7 +14488,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>116</v>
       </c>
@@ -14505,7 +14497,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>117</v>
       </c>
@@ -14514,7 +14506,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
@@ -14523,12 +14515,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>120</v>
       </c>
@@ -14537,7 +14529,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>122</v>
       </c>
@@ -14546,7 +14538,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>123</v>
       </c>
@@ -18600,11 +18592,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="8" width="38.7109375" customWidth="1"/>
@@ -18620,7 +18612,7 @@
     <col min="19" max="19" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
@@ -18666,7 +18658,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="178.5">
+    <row r="3" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>68</v>
       </c>
@@ -18692,15 +18684,15 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q3" s="14"/>
       <c r="R3" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="2:19" ht="63.75">
+    <row r="4" spans="2:19" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>73</v>
@@ -18732,17 +18724,15 @@
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
-      <c r="Q4" s="15" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
       <c r="S4" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="38.25">
+    <row r="5" spans="2:19" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>81</v>
@@ -18774,15 +18764,15 @@
       <c r="P5" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="Q5" s="21" t="s">
-        <v>130</v>
+      <c r="Q5" s="20" t="s">
+        <v>129</v>
       </c>
       <c r="R5" s="15"/>
       <c r="S5" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="2:19" ht="89.25">
+    <row r="6" spans="2:19" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>87</v>
@@ -18815,14 +18805,14 @@
         <v>127</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R6" s="15"/>
       <c r="S6" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="89.25">
+    <row r="7" spans="2:19" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>92</v>
@@ -18852,10 +18842,12 @@
         <v>97</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="Q7" s="15"/>
-      <c r="R7" s="2"/>
+      <c r="R7" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="S7" s="15"/>
     </row>
   </sheetData>
@@ -18877,37 +18869,37 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25">
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5">
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="38.25">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>103</v>
       </c>

</xml_diff>